<commit_message>
page object model added
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Password</t>
   </si>
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,7 +396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -404,48 +404,12 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>